<commit_message>
if no more hints, skip to next round
</commit_message>
<xml_diff>
--- a/Code/data.xlsx
+++ b/Code/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flamu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiaoberhansli/anaconda_projects/Canton-Guessing-Game/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11E641B7-9314-4838-A7D6-B86F8BA5DBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA89D56-3F85-7A4A-8287-EC9253074709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{20D55AB1-3079-44FF-8DF9-39A8F22443C2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{20D55AB1-3079-44FF-8DF9-39A8F22443C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="363">
   <si>
     <t>Canton</t>
   </si>
@@ -1122,6 +1122,9 @@
   </si>
   <si>
     <t>Switzerland's largest city</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
   </si>
 </sst>
 </file>
@@ -1186,7 +1189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1194,11 +1197,489 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1240,476 +1721,6 @@
         </horizontal>
       </border>
     </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1723,37 +1734,54 @@
 </styleSheet>
 </file>
 
+<file path=xl/featurePropertyBag/featurePropertyBag.xml><?xml version="1.0" encoding="utf-8"?>
+<FeaturePropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag">
+  <bag type="Checkbox"/>
+  <bag type="XFControls">
+    <bagId k="CellControl">0</bagId>
+  </bag>
+  <bag type="XFComplement">
+    <bagId k="XFControls">1</bagId>
+  </bag>
+  <bag type="XFComplements" extRef="XFComplementsMapperExtRef">
+    <a k="MappedFeaturePropertyBags">
+      <bagId>2</bagId>
+    </a>
+  </bag>
+</FeaturePropertyBags>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9FD707B0-D478-468B-B445-B4E6F2ECF7FB}" name="Table1" displayName="Table1" ref="A1:T27" totalsRowShown="0" headerRowDxfId="0" dataDxfId="22" headerRowBorderDxfId="1">
-  <autoFilter ref="A1:T27" xr:uid="{9FD707B0-D478-468B-B445-B4E6F2ECF7FB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9FD707B0-D478-468B-B445-B4E6F2ECF7FB}" name="Table1" displayName="Table1" ref="A1:T28" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21">
+  <autoFilter ref="A1:T28" xr:uid="{9FD707B0-D478-468B-B445-B4E6F2ECF7FB}"/>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{FA3D4349-F4F7-4A24-908A-3CF522B63000}" name="Canton" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{4C102336-5DF2-4CBB-ABCC-2E5B815B0888}" name="Population (2022)" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{E18C283C-268A-4324-9D2D-60F22E544769}" name="Capital" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{496624C8-19AB-43DF-A18F-759A78C135F2}" name="Official Language" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{8E9EA0E6-6374-4E17-B487-F47787B21065}" name="Year Joined" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{139359DC-B6E2-4E8C-BCDA-2C15981784D6}" name="Area (km²)" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{121B9D47-DB36-4A35-B757-D9E12A7B9B2F}" name="Highest Point" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{5B839162-6E8B-442F-9C42-0A41BE74F49C}" name="Famous Dish" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{E3147593-1D94-4E8E-B02A-46F233348ACB}" name="Traditional Festival" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{B4A995D4-D22F-445B-B522-3B9E93999E57}" name="Bordering Cantons (names)" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{65E85447-F85B-4742-836C-A2E5AAEC8D9B}" name="Bordering Cantons (no)" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{3DA53440-8715-4118-8EDB-783E9FE87B6A}" name="Famous Person" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{789C1571-AA5D-4FAB-AC82-8587511E0EAA}" name="Notable Landmark" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{5FC1E73C-5C62-4BD0-AB5E-6D5CD0CD7D29}" name="Main Industries" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{B4CDE2BF-7F82-4E56-9913-D12E07A4EE90}" name="UNESCO Heritage" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{F5FA9EA1-9A6D-4A4B-A0A1-C2A49B6B800A}" name="Lake/River" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{960F2CBE-A197-4976-A14F-311059579F89}" name="Mountain Pass" dataDxfId="5"/>
-    <tableColumn id="18" xr3:uid="{1AD715A9-6507-4E5F-99BC-52CCC9CD046E}" name="Nickname" dataDxfId="4"/>
-    <tableColumn id="19" xr3:uid="{FF27E968-908A-4D06-8805-62386D4CC7BF}" name="Traditional Costume" dataDxfId="3"/>
-    <tableColumn id="20" xr3:uid="{F5BC11BF-2BC0-494E-B2F4-9E82522234EF}" name="Unique Fact" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{FA3D4349-F4F7-4A24-908A-3CF522B63000}" name="Canton" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{4C102336-5DF2-4CBB-ABCC-2E5B815B0888}" name="Population (2022)" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{E18C283C-268A-4324-9D2D-60F22E544769}" name="Capital" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{496624C8-19AB-43DF-A18F-759A78C135F2}" name="Official Language" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{8E9EA0E6-6374-4E17-B487-F47787B21065}" name="Year Joined" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{139359DC-B6E2-4E8C-BCDA-2C15981784D6}" name="Area (km²)" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{121B9D47-DB36-4A35-B757-D9E12A7B9B2F}" name="Highest Point" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{5B839162-6E8B-442F-9C42-0A41BE74F49C}" name="Famous Dish" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{E3147593-1D94-4E8E-B02A-46F233348ACB}" name="Traditional Festival" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{B4A995D4-D22F-445B-B522-3B9E93999E57}" name="Bordering Cantons (names)" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{65E85447-F85B-4742-836C-A2E5AAEC8D9B}" name="Bordering Cantons (no)" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{3DA53440-8715-4118-8EDB-783E9FE87B6A}" name="Famous Person" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{789C1571-AA5D-4FAB-AC82-8587511E0EAA}" name="Notable Landmark" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{5FC1E73C-5C62-4BD0-AB5E-6D5CD0CD7D29}" name="Main Industries" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{B4CDE2BF-7F82-4E56-9913-D12E07A4EE90}" name="UNESCO Heritage" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{F5FA9EA1-9A6D-4A4B-A0A1-C2A49B6B800A}" name="Lake/River" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{960F2CBE-A197-4976-A14F-311059579F89}" name="Mountain Pass" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{1AD715A9-6507-4E5F-99BC-52CCC9CD046E}" name="Nickname" dataDxfId="2"/>
+    <tableColumn id="19" xr3:uid="{FF27E968-908A-4D06-8805-62386D4CC7BF}" name="Traditional Costume" dataDxfId="1"/>
+    <tableColumn id="20" xr3:uid="{F5BC11BF-2BC0-494E-B2F4-9E82522234EF}" name="Unique Fact" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2069,39 +2097,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2172FE-848C-45D8-A041-48C9D06BAE56}">
-  <dimension ref="A1:T27"/>
+  <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
-    <col min="10" max="10" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" customWidth="1"/>
     <col min="11" max="11" width="24" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" customWidth="1"/>
+    <col min="13" max="13" width="19.5" customWidth="1"/>
     <col min="14" max="14" width="17" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" customWidth="1"/>
-    <col min="19" max="19" width="21.42578125" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" customWidth="1"/>
+    <col min="15" max="15" width="19.1640625" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" customWidth="1"/>
+    <col min="17" max="17" width="16.1640625" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" customWidth="1"/>
+    <col min="19" max="19" width="21.5" customWidth="1"/>
+    <col min="20" max="20" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -2162,139 +2190,139 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="120" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2">
+        <v>4</v>
+      </c>
+      <c r="I2" s="2">
+        <v>3</v>
+      </c>
+      <c r="J2" s="2">
+        <v>5</v>
+      </c>
+      <c r="K2" s="2">
+        <v>4</v>
+      </c>
+      <c r="L2" s="2">
+        <v>6</v>
+      </c>
+      <c r="M2" s="2">
+        <v>7</v>
+      </c>
+      <c r="N2" s="2">
+        <v>5</v>
+      </c>
+      <c r="O2" s="2">
+        <v>6</v>
+      </c>
+      <c r="P2" s="2">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>6</v>
+      </c>
+      <c r="R2" s="2">
+        <v>7</v>
+      </c>
+      <c r="S2" s="2">
+        <v>9</v>
+      </c>
+      <c r="T2" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1803</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" s="1">
-        <v>6</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E3" s="1">
-        <v>1513</v>
-      </c>
-      <c r="F3" s="1">
-        <v>243</v>
+        <v>1803</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="K3" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>23</v>
@@ -2303,19 +2331,19 @@
         <v>1513</v>
       </c>
       <c r="F4" s="1">
-        <v>173</v>
+        <v>243</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="K4" s="1">
         <v>2</v>
@@ -2324,10 +2352,10 @@
         <v>44</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>32</v>
@@ -2339,119 +2367,119 @@
         <v>32</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E5" s="1">
-        <v>1833</v>
+        <v>1513</v>
       </c>
       <c r="F5" s="1">
-        <v>518</v>
+        <v>173</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="K5" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>32</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>32</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="1">
-        <v>1501</v>
+        <v>1833</v>
       </c>
       <c r="F6" s="1">
-        <v>37</v>
+        <v>518</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="K6" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>82</v>
+        <v>31</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>32</v>
@@ -2463,582 +2491,582 @@
         <v>32</v>
       </c>
       <c r="R6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1501</v>
+      </c>
+      <c r="F7" s="1">
+        <v>37</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R7" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E8" s="1">
         <v>1353</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K8" s="1">
         <v>11</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="T8" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E9" s="1">
         <v>1481</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K9" s="1">
         <v>4</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="Q8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R8" s="1" t="s">
+      <c r="Q9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R9" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E10" s="1">
         <v>1815</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F10" s="1">
         <v>282</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K10" s="1">
         <v>2</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P9" s="1" t="s">
+      <c r="O10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="Q9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R9" s="1" t="s">
+      <c r="Q10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R10" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="S10" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="T10" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E11" s="1">
         <v>1352</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F11" s="1">
         <v>685</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="I11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K11" s="1">
         <v>4</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P10" s="1" t="s">
+      <c r="O11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q11" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="R11" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="S11" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="T11" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E12" s="1">
         <v>1803</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K12" s="1">
         <v>5</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="O12" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q12" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S11" s="1" t="s">
+      <c r="S12" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="T12" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="105" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E13" s="1">
         <v>1979</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F13" s="1">
         <v>838</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J12" s="1" t="s">
+      <c r="I13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K13" s="1">
         <v>4</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P12" s="1" t="s">
+      <c r="O13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="Q12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R12" s="1" t="s">
+      <c r="Q13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R13" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="S13" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="T13" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E14" s="1">
         <v>1332</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K14" s="1">
         <v>6</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="O13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P13" s="1" t="s">
+      <c r="O14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P14" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="Q14" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="R13" s="1" t="s">
+      <c r="R14" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="S13" s="1" t="s">
+      <c r="S14" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="T13" s="1" t="s">
+      <c r="T14" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E15" s="1">
         <v>1815</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F15" s="1">
         <v>803</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="K14" s="1">
-        <v>4</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1291</v>
-      </c>
-      <c r="F15" s="1">
-        <v>276</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="K15" s="1">
         <v>4</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>44</v>
+        <v>192</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>205</v>
+        <v>167</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>32</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>32</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>23</v>
@@ -3047,19 +3075,19 @@
         <v>1291</v>
       </c>
       <c r="F16" s="1">
-        <v>491</v>
+        <v>276</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>32</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="K16" s="1">
         <v>4</v>
@@ -3068,287 +3096,287 @@
         <v>44</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>57</v>
+        <v>205</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>32</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>216</v>
+        <v>181</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>182</v>
+        <v>32</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="1">
-        <v>1501</v>
+        <v>1291</v>
       </c>
       <c r="F17" s="1">
-        <v>298</v>
+        <v>491</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="K17" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>225</v>
+        <v>44</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>227</v>
+        <v>57</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>70</v>
+        <v>216</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>32</v>
+        <v>182</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="105" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E18" s="1">
-        <v>1291</v>
+        <v>1501</v>
       </c>
       <c r="F18" s="1">
-        <v>908</v>
+        <v>298</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>32</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="K18" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>205</v>
+        <v>227</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>32</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>238</v>
+        <v>70</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>239</v>
+        <v>32</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="1">
-        <v>1481</v>
+        <v>1291</v>
       </c>
       <c r="F19" s="1">
-        <v>790</v>
+        <v>908</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>32</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="K19" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>250</v>
+        <v>205</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>32</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>33</v>
+        <v>238</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>32</v>
+        <v>239</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="150" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E20" s="1">
-        <v>1803</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>256</v>
+        <v>1481</v>
+      </c>
+      <c r="F20" s="1">
+        <v>790</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>259</v>
+        <v>32</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="K20" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>138</v>
+        <v>250</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>263</v>
+        <v>32</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>264</v>
+        <v>33</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>32</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>23</v>
@@ -3356,35 +3384,35 @@
       <c r="E21" s="1">
         <v>1803</v>
       </c>
-      <c r="F21" s="1">
-        <v>992</v>
+      <c r="F21" s="1" t="s">
+        <v>256</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>32</v>
+        <v>259</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="K21" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>44</v>
+        <v>261</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>205</v>
+        <v>138</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>32</v>
+        <v>263</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>264</v>
@@ -3393,384 +3421,446 @@
         <v>32</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>278</v>
+        <v>244</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>280</v>
+        <v>23</v>
       </c>
       <c r="E22" s="1">
         <v>1803</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>281</v>
+      <c r="F22" s="1">
+        <v>992</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>32</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="K22" s="1">
         <v>3</v>
       </c>
       <c r="L22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1803</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="K23" s="1">
+        <v>3</v>
+      </c>
+      <c r="L23" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="M23" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="N22" s="1" t="s">
+      <c r="N23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="O23" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="P23" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="Q22" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="150" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="1">
-        <v>1291</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="K23" s="1">
-        <v>7</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>288</v>
       </c>
       <c r="R23" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1291</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="K24" s="1">
+        <v>7</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="R24" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="S23" s="1" t="s">
+      <c r="S24" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="T23" s="1" t="s">
+      <c r="T24" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E25" s="1">
         <v>1815</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K25" s="1">
         <v>4</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="M25" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="N24" s="1" t="s">
+      <c r="N25" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="O24" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="P24" s="1" t="s">
+      <c r="P25" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="Q24" s="1" t="s">
+      <c r="Q25" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="R24" s="1" t="s">
+      <c r="R25" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="S24" s="1" t="s">
+      <c r="S25" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="T24" s="1" t="s">
+      <c r="T25" s="1" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E26" s="1">
         <v>1803</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K26" s="1">
         <v>5</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="M26" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="N25" s="1" t="s">
+      <c r="N26" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="O26" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="P25" s="1" t="s">
+      <c r="P26" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="Q26" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="R25" s="1" t="s">
+      <c r="R26" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="S25" s="1" t="s">
+      <c r="S26" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="T25" s="1" t="s">
+      <c r="T26" s="1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>338</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="1">
-        <v>1352</v>
-      </c>
-      <c r="F26" s="1">
-        <v>239</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="K26" s="1">
-        <v>4</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="Q26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="S26" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="T26" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" ht="120" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>349</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E27" s="1">
+        <v>1352</v>
+      </c>
+      <c r="F27" s="1">
+        <v>239</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="K27" s="1">
+        <v>4</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="1">
         <v>1351</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K28" s="1">
         <v>6</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="M28" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="N27" s="1" t="s">
+      <c r="N28" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="O27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P27" s="1" t="s">
+      <c r="O28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P28" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="Q27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R27" s="1" t="s">
+      <c r="Q28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R28" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="S27" s="1" t="s">
+      <c r="S28" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="T27" s="1" t="s">
+      <c r="T28" s="1" t="s">
         <v>361</v>
       </c>
     </row>

</xml_diff>